<commit_message>
GPU/CPU 加速12倍 ， 矩阵求逆1536*1536
</commit_message>
<xml_diff>
--- a/NVIDIA_CUDA-5.0_Samples/8_diy/matrixInv/性能测试.xlsx
+++ b/NVIDIA_CUDA-5.0_Samples/8_diy/matrixInv/性能测试.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>数据大小</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -72,6 +72,14 @@
   </si>
   <si>
     <t>s --&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CPU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPG/CPU</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -472,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:L16"/>
+  <dimension ref="B3:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -696,6 +704,23 @@
       </c>
       <c r="I16" s="7" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="8:9">
+      <c r="H18" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="8:9">
+      <c r="H19" t="s">
+        <v>18</v>
+      </c>
+      <c r="I19">
+        <f>I18/I12</f>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>